<commit_message>
Add option modification in game
</commit_message>
<xml_diff>
--- a/Matrice.xlsx
+++ b/Matrice.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Unity\TowerDefense\TowerDefense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6594055-7605-4BF2-98FC-4D276C093E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F30B2-71DA-4C73-8C2E-164040560E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8DAE865-095E-4013-A252-09D959A0DC8F}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E8DAE865-095E-4013-A252-09D959A0DC8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Towers" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Goblin</t>
   </si>
@@ -48,6 +49,27 @@
   </si>
   <si>
     <t>Experience</t>
+  </si>
+  <si>
+    <t>dps</t>
+  </si>
+  <si>
+    <t>Eye</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
+    <t>50/70</t>
+  </si>
+  <si>
+    <t>NbrSprite</t>
+  </si>
+  <si>
+    <t>Vitesse</t>
+  </si>
+  <si>
+    <t>HP</t>
   </si>
 </sst>
 </file>
@@ -83,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,52 +450,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9E1E02-E78D-4C99-99BC-D75F0AB9F9B6}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>50.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>B2*(B9/B8)</f>
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <f>C2*(C9/C8)</f>
+        <v>34.61538461538462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80DCAEB-3550-4AA1-B1D0-74884108736C}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Warchief + bosswave system
</commit_message>
<xml_diff>
--- a/Matrice.xlsx
+++ b/Matrice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Unity\TowerDefense\TowerDefense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F30B2-71DA-4C73-8C2E-164040560E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0329E10E-D9B2-4DE6-A4FD-C4782329F7DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E8DAE865-095E-4013-A252-09D959A0DC8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Goblin</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>HP</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>King</t>
   </si>
 </sst>
 </file>
@@ -568,26 +583,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80DCAEB-3550-4AA1-B1D0-74884108736C}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>